<commit_message>
2.04a bugfix + 2.05 developmental bits
</commit_message>
<xml_diff>
--- a/doc/nfs4_perms_cribsheet.xlsx
+++ b/doc/nfs4_perms_cribsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="2040" windowWidth="24500" windowHeight="17400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ACL Permissions" sheetId="1" r:id="rId1"/>
@@ -785,6 +785,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (full access)</t>
@@ -800,6 +801,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (modify access)</t>
@@ -815,6 +817,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read and execute access)</t>
@@ -830,6 +833,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read-only access)</t>
@@ -845,6 +849,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write-only access)</t>
@@ -860,6 +865,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (delete)</t>
@@ -875,6 +881,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read control)</t>
@@ -890,6 +897,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write DAC)</t>
@@ -905,6 +913,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write owner)</t>
@@ -920,6 +929,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (synchronize)</t>
@@ -935,6 +945,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (access system security)</t>
@@ -950,6 +961,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (maximum allowed)</t>
@@ -965,6 +977,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (generic read)</t>
@@ -980,6 +993,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (generic write)</t>
@@ -995,6 +1009,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (generic execute)</t>
@@ -1010,6 +1025,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (generic all)</t>
@@ -1025,6 +1041,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read data/list directory)</t>
@@ -1040,6 +1057,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write data/add file)</t>
@@ -1055,6 +1073,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (append data/add subdirectory)</t>
@@ -1070,6 +1089,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read extended attributes)</t>
@@ -1085,6 +1105,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write extended attributes)</t>
@@ -1100,6 +1121,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (execute/traverse)</t>
@@ -1115,6 +1137,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (delete child)</t>
@@ -1130,6 +1153,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (read attributes)</t>
@@ -1145,6 +1169,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (write attributes)</t>
@@ -1242,6 +1267,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1884,7 +1910,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2035,6 +2061,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2522,7 +2551,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="182">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2626,6 +2655,9 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3033,8 +3065,8 @@
   <dimension ref="A1:AH154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="6" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A131" sqref="A131:XFD131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8959,7 +8991,7 @@
     </row>
     <row r="131" spans="1:34">
       <c r="A131" s="115" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B131" s="147" t="s">
         <v>200</v>
@@ -9009,7 +9041,7 @@
     </row>
     <row r="132" spans="1:34">
       <c r="A132" s="115" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B132" s="147" t="s">
         <v>294</v>
@@ -9055,7 +9087,7 @@
       <c r="AG132" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AH132" s="14" t="s">
+      <c r="AH132" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -10058,9 +10090,9 @@
       <c r="AH154" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A127:AH136">
-    <sortCondition ref="B127:B136"/>
-    <sortCondition ref="A127:A136"/>
+  <sortState ref="A129:AH136">
+    <sortCondition ref="B129:B136"/>
+    <sortCondition ref="A129:A136"/>
   </sortState>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
@@ -10084,7 +10116,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>